<commit_message>
fix wire color mistake
</commit_message>
<xml_diff>
--- a/Teensy4.0_STM32_Mapping.xlsx
+++ b/Teensy4.0_STM32_Mapping.xlsx
@@ -435,92 +435,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -916,8 +847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L39" sqref="L39"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,68 +888,68 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="8" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="5" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="8" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -1030,7 +961,7 @@
       <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="7" t="s">
         <v>50</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -1060,7 +991,7 @@
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="6"/>
+      <c r="D7" s="8"/>
       <c r="E7" s="4" t="s">
         <v>11</v>
       </c>
@@ -1088,7 +1019,7 @@
       <c r="C8" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="8" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="4" t="s">
@@ -1118,7 +1049,7 @@
       <c r="C9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="6"/>
+      <c r="D9" s="8"/>
       <c r="E9" s="4" t="s">
         <v>11</v>
       </c>
@@ -1388,7 +1319,7 @@
         <v>84</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -1415,7 +1346,7 @@
         <v>85</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -1868,44 +1799,44 @@
     <mergeCell ref="D8:D9"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:H1048576 O6:O18">
-    <cfRule type="containsText" dxfId="20" priority="13" operator="containsText" text="Black">
+    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="Black">
       <formula>NOT(ISERROR(SEARCH("Black",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="14" operator="containsText" text="Brown">
+    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="Brown">
       <formula>NOT(ISERROR(SEARCH("Brown",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="15" operator="containsText" text="Grey">
+    <cfRule type="containsText" dxfId="9" priority="15" operator="containsText" text="Grey">
       <formula>NOT(ISERROR(SEARCH("Grey",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="Blue">
+    <cfRule type="containsText" dxfId="8" priority="16" operator="containsText" text="Blue">
       <formula>NOT(ISERROR(SEARCH("Blue",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="Red">
+    <cfRule type="containsText" dxfId="7" priority="17" operator="containsText" text="Red">
       <formula>NOT(ISERROR(SEARCH("Red",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="Orange">
+    <cfRule type="containsText" dxfId="6" priority="18" operator="containsText" text="Orange">
       <formula>NOT(ISERROR(SEARCH("Orange",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="19" operator="containsText" text="Purple">
+    <cfRule type="containsText" dxfId="5" priority="19" operator="containsText" text="Purple">
       <formula>NOT(ISERROR(SEARCH("Purple",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="20" operator="containsText" text="Yellow">
+    <cfRule type="containsText" dxfId="4" priority="20" operator="containsText" text="Yellow">
       <formula>NOT(ISERROR(SEARCH("Yellow",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="21" operator="containsText" text="Green">
+    <cfRule type="containsText" dxfId="3" priority="21" operator="containsText" text="Green">
       <formula>NOT(ISERROR(SEARCH("Green",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="11" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6:F38">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G38">
-    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576">

</xml_diff>

<commit_message>
permanent wiring - SerialST4 not working
</commit_message>
<xml_diff>
--- a/Teensy4.0_STM32_Mapping.xlsx
+++ b/Teensy4.0_STM32_Mapping.xlsx
@@ -850,8 +850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,7 +906,7 @@
         <v>113</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>115</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -942,7 +942,7 @@
         <v>114</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1643,7 +1643,7 @@
         <v>14</v>
       </c>
       <c r="F34" s="3" t="str">
-        <f>IF(B34=E34,"","X")</f>
+        <f t="shared" ref="F34:F40" si="1">IF(B34=E34,"","X")</f>
         <v>X</v>
       </c>
       <c r="G34" s="2" t="s">
@@ -1670,7 +1670,7 @@
         <v>15</v>
       </c>
       <c r="F35" s="3" t="str">
-        <f>IF(B35=E35,"","X")</f>
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="G35" s="2" t="s">
@@ -1697,7 +1697,7 @@
         <v>16</v>
       </c>
       <c r="F36" s="3" t="str">
-        <f>IF(B36=E36,"","X")</f>
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="G36" s="2" t="s">
@@ -1724,7 +1724,7 @@
         <v>17</v>
       </c>
       <c r="F37" s="3" t="str">
-        <f>IF(B37=E37,"","X")</f>
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="G37" s="2" t="s">
@@ -1751,7 +1751,7 @@
         <v>18</v>
       </c>
       <c r="F38" s="3" t="str">
-        <f>IF(B38=E38,"","X")</f>
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="G38" s="2" t="s">
@@ -1778,7 +1778,7 @@
         <v>20</v>
       </c>
       <c r="F39" s="3" t="str">
-        <f>IF(B39=E39,"","X")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G39" s="2" t="s">
@@ -1805,7 +1805,7 @@
         <v>21</v>
       </c>
       <c r="F40" s="3" t="str">
-        <f>IF(B40=E40,"","X")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G40" s="2" t="s">

</xml_diff>